<commit_message>
Add more financial information to expenses and revenues tracking
Update ExcelStorage class to include baseAmount, GST, HSN, invoice, and currency columns in expenses and revenues.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: cdd29b5b-2652-4b10-9df1-39d8388fd989
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7193f0d6-a227-4876-829b-be28091fbb85/33f4bcab-8075-40cf-91a0-2c674ab4b6de.jpg
</commit_message>
<xml_diff>
--- a/data/production_units.xlsx
+++ b/data/production_units.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Production Units" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>createdAt</t>
+  </si>
+  <si>
+    <t>Sample Production Unit</t>
+  </si>
+  <si>
+    <t>Delhi, India</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2025-05-05T08:47:19.803Z</t>
   </si>
 </sst>
 </file>
@@ -419,12 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="4" width="10" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -445,6 +463,26 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>